<commit_message>
correct layer-id, file references for hv site, and update fields description files
</commit_message>
<xml_diff>
--- a/fields_description/high_volume_receiving_sites.xlsx
+++ b/fields_description/high_volume_receiving_sites.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28014"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB_REPOS\nr-soils-relocation\fields_description\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8DCCD5-BDE6-4753-9716-CE80AB92CC3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{9A8DCCD5-BDE6-4753-9716-CE80AB92CC3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FDE45D9-A7FE-4713-91E7-8D429EDB1C6C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,136 +36,163 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+  <si>
+    <t>field</t>
+  </si>
+  <si>
+    <t>long desc</t>
+  </si>
   <si>
     <t>confirmationId</t>
   </si>
   <si>
+    <t>The confirmation ID is a number generated by the CHEFS form each time a soil relocation notification form is submitted. The number is used by submitters, First Nations, municipalities, members of the public and ministry staff to track individual submissions. The confirmation ID can also be used to request additional information from the soil relocation team. It is not editable.</t>
+  </si>
+  <si>
     <t>ownerCompany</t>
   </si>
   <si>
+    <t>The field records the name of the company associated with the property owner of the high volume soil receiving site. An example entry might be 'South Coast British Columbia Transportation Authority, TransLink.' The data is in a nullable text format.</t>
+  </si>
+  <si>
     <t>owner2Company</t>
   </si>
   <si>
+    <t>The field records the name of an additional company associated with the property owner of the high volume soil receiving site. An example entry might be '359719 B.C. LTD.' The data is in a nullable text format.</t>
+  </si>
+  <si>
     <t>contactCompany</t>
   </si>
   <si>
+    <t>The field records the name of the company associated with the contact person for the high volume soil receiving site. An example entry might be 'Summit Earthworks Inc.' The data is in a nullable text format.</t>
+  </si>
+  <si>
     <t>SID</t>
   </si>
   <si>
+    <t xml:space="preserve">The field displays the Site registry number which users enter into the High Volume Receiving Site Registration form if their property has a Site registry site ID. The site ID is a numerical value and can be a single digit or up to 5 digits in length.  </t>
+  </si>
+  <si>
     <t>latitude</t>
   </si>
   <si>
+    <t>The field records the latitude of the high volume soil receiving site. An example entry might be '49.2687277777777.' The data is in a nullable Double format.</t>
+  </si>
+  <si>
     <t>longitude</t>
   </si>
   <si>
+    <t>The field records the longitude of the high volume soil receiving  site. An example entry might be '-123.002644444444.' The data is in a nullable Double format.</t>
+  </si>
+  <si>
+    <t>regionalDistrict</t>
+  </si>
+  <si>
+    <t>The field records the regional district of the high volume soil receiving site. The data is a non-nullable text type. For example, 'Metro Vancouver Regional District.' is one of selections.</t>
+  </si>
+  <si>
     <t>landOwnership</t>
   </si>
   <si>
+    <t>The field indicates the type of land ownership for the high volume soil receiving  site. The data is in text format, with the complete list of options being 'Legally titled, registered property', 'Untitled Crown land', 'Untitled municipal land', or 'Reserve land.'</t>
+  </si>
+  <si>
     <t>legallyTitledSiteAddress</t>
   </si>
   <si>
+    <t>The field records the site street address for a legally titled, registered property of the high volume soil receiving site. If an address is not assigned, the nearest street name or intersection should be provided. The data is in nullable text format, and an example entry might be '4567 Lougheed Highway.'</t>
+  </si>
+  <si>
     <t>legallyTitledSiteCity</t>
   </si>
   <si>
+    <t>The field records the site city for a legally titled, registered property of the high volume soil receiving site. The data is in nullable text format, and an example entry might be 'Burnaby.'</t>
+  </si>
+  <si>
     <t>legallyTitledSitePostalCode</t>
   </si>
   <si>
-    <t>regionalDistrict</t>
+    <t>The field records the site postal code for a legally titled, registered property of the high volume soil receiving site. The data is in nullable text format, and an example entry might be 'V5C 3Z6.'</t>
   </si>
   <si>
     <t>PID</t>
   </si>
   <si>
+    <t>The field records the Parcel Identifier (PID) for each parcel at the high volume soil receiving site where a Schedule 2 use has occurred. PIDs can be found on BC Assessment or the BC Land Title and Survey Authority (LTSA). The data format is 'XXX-XXX-XXX,' where each 'X' is a digit. If the site has multiple PIDs, they will be represented as a comma-separated list. An example entry might be '013-206-222,008-238-057,011-263-873,013-038-796,009-324-532' or '032-275-161.' The data is in a nullable String format.</t>
+  </si>
+  <si>
     <t>PIN</t>
   </si>
   <si>
+    <t>The field records the Parcel Identification Number (PIN) for untitled Crown land of the high volume soil receiving site involved in the soil relocation. The data is in a nullable text format, and an example entry might be '7126700.'</t>
+  </si>
+  <si>
     <t>legalLandDescription</t>
   </si>
   <si>
+    <t>The field lists the unique legal description of the property, usually consisting of a lot or parcel number, other identifiers and a plan number.  The legal land description can be obtained through the BC Land Title and Survey Authority (LTSA).</t>
+  </si>
+  <si>
     <t>crownLandFileNumbers</t>
   </si>
   <si>
+    <t>The field records the file number(s) for untitled Crown land of the high volume soil receiving site. The data is in a nullable text format.</t>
+  </si>
+  <si>
     <t>reserveNameAndNumber</t>
   </si>
   <si>
+    <t xml:space="preserve">The field displays the First Nation Reserve name and number for those receiving sites that are on First Nation Reserves. </t>
+  </si>
+  <si>
+    <t>receivingSiteLandUse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The field displays the applicable primary land use for the receiving site as per the Contaminated Sites Regulations Section 12.  Submitters consider current and future use of the receiving site land. </t>
+  </si>
+  <si>
+    <t>hvsConfirmation</t>
+  </si>
+  <si>
+    <t>The field records whether the receiving site qualifies as a high volume site, defined as having more than 20,000 cubic metres of material deposited over its lifetime. The data is stored as 'Yes' or 'No', ensuring accurate classification of the site's volume status for tracking and regulatory purposes.</t>
+  </si>
+  <si>
+    <t>dateSiteBecameHighVolume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The field displays the total volume of commercial and/or industrial quality soil received at the site surpassed 20,000 cubic metres.  The data is in DATE format. </t>
+  </si>
+  <si>
+    <t>howRelocatedSoilWillBeUsed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The field displays how the relocated soil will be used at the receiving site, for example fill, cover, berms.  The format is a nullable text entry. </t>
+  </si>
+  <si>
+    <t>soilDepositIsALR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The field records whether the receiving site is part of the Agricultural Land Reserve (ALR).  The box is selected if the answer is yes.  Submitters are directed to inform the Agricultural Land commission (ALC) </t>
+  </si>
+  <si>
+    <t>soilDepositIsReserveLands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The field records whether the receiving site is located on a First Nation Reserve.  The box is selected if the answer is yes.  Submitters are directed to inform Indigenous Services Canada. </t>
+  </si>
+  <si>
     <t>qualifiedProfessionalOrganization</t>
   </si>
   <si>
-    <t>field</t>
-  </si>
-  <si>
-    <t>long desc</t>
-  </si>
-  <si>
-    <t>receivingSiteLandUse</t>
-  </si>
-  <si>
-    <t>hvsConfirmation</t>
-  </si>
-  <si>
-    <t>dateSiteBecameHighVolume</t>
-  </si>
-  <si>
-    <t>howRelocatedSoilWillBeUsed</t>
-  </si>
-  <si>
-    <t>soilDepositIsALR</t>
-  </si>
-  <si>
-    <t>soilDepositIsReserveLands</t>
-  </si>
-  <si>
-    <t>The confirmation ID is a number generated by the CHEFS form each time a soil relocation notification form is submitted. The number is used by submitters, First Nations, municipalities, members of the public and ministry staff to track individual submissions. The confirmation ID can also be used to request additional information from the soil relocation team. It is not editable.</t>
-  </si>
-  <si>
-    <t>The field records the name of the company associated with the property owner of the source site involved in the soil relocation. An example entry might be 'South Coast British Columbia Transportation Authority, TransLink.' The data is in a nullable text format.</t>
-  </si>
-  <si>
-    <t>The field records the name of an additional company associated with the property owner of the source site involved in the soil relocation, if applicable. An example entry might be '359719 B.C. LTD.' The data is in a nullable text format.</t>
-  </si>
-  <si>
     <t>The field records the name of the organization associated with the qualified professional overseeing the soil relocation process. An example entry might be 'WSP Canada Inc.'. It is an nullable text entry.</t>
-  </si>
-  <si>
-    <t>The field records the name of the company associated with the contact person for the high volume soil receiving site. An example entry might be 'Summit Earthworks Inc.' The data is in a nullable text format.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The field displays the Site registry number which users enter into the soil relocation submission form if their property has a Site registry site ID. The site ID is a numerical value and can be a single digit or up to 5 digits in length.  </t>
-  </si>
-  <si>
-    <t>The field records the latitude of the high volume soil receiving site. An example entry might be '49.2687277777777.' The data is in a nullable Double format.</t>
-  </si>
-  <si>
-    <t>The field records the longitude of the high volume soil receiving  site. An example entry might be '-123.002644444444.' The data is in a nullable Double format.</t>
-  </si>
-  <si>
-    <t>The field records the regional district of the high volume soil receiving site. The data is a non-nullable text type. For example, 'Metro Vancouver Regional District.' is one of selections.</t>
-  </si>
-  <si>
-    <t>The field indicates the type of land ownership for the high volume soil receiving  site. The data is in text format, with the complete list of options being 'Legally titled, registered property', 'Untitled Crown land', 'Untitled municipal land', or 'Reserve land.'</t>
-  </si>
-  <si>
-    <t>The field records the site street address for a legally titled, registered property of the high volume soil receiving site. If an address is not assigned, the nearest street name or intersection should be provided. The data is in nullable text format, and an example entry might be '4567 Lougheed Highway.'</t>
-  </si>
-  <si>
-    <t>The field records the site city for a legally titled, registered property of the high volume soil receiving site. The data is in nullable text format, and an example entry might be 'Burnaby.'</t>
-  </si>
-  <si>
-    <t>The field records the site postal code for a legally titled, registered property of the high volume soil receiving site. The data is in nullable text format, and an example entry might be 'V5C 3Z6.'</t>
-  </si>
-  <si>
-    <t>The field records the Parcel Identifier (PID) for each parcel at the high volume soil receiving site where a Schedule 2 use has occurred. PIDs can be found on BC Assessment or the BC Land Title and Survey Authority (LTSA). The data format is 'XXX-XXX-XXX,' where each 'X' is a digit. If the site has multiple PIDs, they will be represented as a comma-separated list. An example entry might be '013-206-222,008-238-057,011-263-873,013-038-796,009-324-532' or '032-275-161.' The data is in a nullable String format.</t>
-  </si>
-  <si>
-    <t>The field records the Parcel Identification Number (PIN) for untitled Crown land of the high volume soil receiving site involved in the soil relocation. The data is in a nullable text format, and an example entry might be '7126700.'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -557,188 +584,214 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30.42578125" customWidth="1"/>
     <col min="2" max="2" width="128.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B14" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="15" spans="1:2">
+      <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="B16" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="B17" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="18" spans="1:2">
+      <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="B18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="B19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="B20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="21" spans="1:2">
+      <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="29.25">
       <c r="A23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update field name in excel - 'qualifiedProfessionalOrganizati' is actual name of the field in AGOL internally rather than 'qualifiedProfessionalOrganization'
</commit_message>
<xml_diff>
--- a/fields_description/high_volume_receiving_sites.xlsx
+++ b/fields_description/high_volume_receiving_sites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB_REPOS\nr-soils-relocation\fields_description\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{9A8DCCD5-BDE6-4753-9716-CE80AB92CC3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FDE45D9-A7FE-4713-91E7-8D429EDB1C6C}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{9A8DCCD5-BDE6-4753-9716-CE80AB92CC3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E8E7B5C-C666-41A5-864D-0A25DED20C04}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,6 +35,22 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Roy Jeong</author>
+  </authors>
+  <commentList>
+    <comment ref="A25" authorId="0" shapeId="0" xr:uid="{CBC12D9E-16B8-4477-999B-5E8BEED17DCC}">
+      <text>
+        <t>Roy Jeong:
+Never rename fields. The field name is not incorrect, it is currently actually referenced as such in AGOL internally.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
@@ -182,7 +198,7 @@
     <t xml:space="preserve">The field records whether the receiving site is located on a First Nation Reserve.  The box is selected if the answer is yes.  Submitters are directed to inform Indigenous Services Canada. </t>
   </si>
   <si>
-    <t>qualifiedProfessionalOrganization</t>
+    <t>qualifiedProfessionalOrganizati</t>
   </si>
   <si>
     <t>The field records the name of the organization associated with the qualified professional overseeing the soil relocation process. An example entry might be 'WSP Canada Inc.'. It is an nullable text entry.</t>
@@ -581,11 +597,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -796,5 +812,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>